<commit_message>
update date and hour
</commit_message>
<xml_diff>
--- a/VTR_DINOTRENT01_VALUES_XML_022522.xlsx
+++ b/VTR_DINOTRENT01_VALUES_XML_022522.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25023"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgallego/Dropbox (ELC)/CONTENT_OPS/FORMATTED_METADATA/VTR_METADATA_XML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D6B2D17-DDAF-4B87-8023-B2A68D678C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA121F6A-8926-41B7-A5EC-1AF7C6A17C54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="16640" windowHeight="17320" firstSheet="1" activeTab="1" xr2:uid="{03BED2AC-B7EF-AB4D-9CDB-0EAAF21C9506}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{03BED2AC-B7EF-AB4D-9CDB-0EAAF21C9506}"/>
   </bookViews>
   <sheets>
     <sheet name="DINOTREN_T01-SD_ADI.XML" sheetId="6" r:id="rId1"/>
@@ -24,10 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>FileName</t>
   </si>
@@ -332,16 +328,23 @@
   </si>
   <si>
     <t>EEDITR102.ts</t>
+  </si>
+  <si>
+    <t>DINOTREN_T01-SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>DINOTREN_T02-SD_ADI.XML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +396,13 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,90 +459,94 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="21" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,7 +563,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -847,425 +861,433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92B4645-07E8-BF4B-BEED-9FC41AEB87DF}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD23"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="16.875" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="21.875" customWidth="1"/>
-    <col min="9" max="9" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.625" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="22.125" customWidth="1"/>
-    <col min="14" max="14" width="28.125" customWidth="1"/>
-    <col min="16" max="17" width="31.625" customWidth="1"/>
-    <col min="18" max="18" width="15.125" customWidth="1"/>
-    <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="21" max="21" width="22.125" customWidth="1"/>
-    <col min="22" max="22" width="18.875" customWidth="1"/>
-    <col min="23" max="23" width="15.625" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.5" customWidth="1"/>
-    <col min="26" max="26" width="23" customWidth="1"/>
-    <col min="27" max="29" width="16" customWidth="1"/>
-    <col min="30" max="30" width="25.875" customWidth="1"/>
-    <col min="31" max="31" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.625" customWidth="1"/>
-    <col min="33" max="33" width="16.625" customWidth="1"/>
-    <col min="34" max="34" width="19" customWidth="1"/>
-    <col min="35" max="36" width="28.875" customWidth="1"/>
-    <col min="37" max="37" width="14.375" customWidth="1"/>
-    <col min="40" max="42" width="15.5" customWidth="1"/>
-    <col min="43" max="43" width="16.375" customWidth="1"/>
-    <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="45.375" customWidth="1"/>
-    <col min="48" max="48" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="34.125" customWidth="1"/>
-    <col min="52" max="52" width="19" customWidth="1"/>
-    <col min="53" max="53" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="32" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="11" style="19"/>
+    <col min="4" max="4" width="13.375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="21" style="19" customWidth="1"/>
+    <col min="6" max="6" width="16.875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="21.875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="22.875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="26" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="19" customWidth="1"/>
+    <col min="13" max="13" width="22.125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="28.125" style="19" customWidth="1"/>
+    <col min="15" max="15" width="11" style="19"/>
+    <col min="16" max="17" width="31.625" style="19" customWidth="1"/>
+    <col min="18" max="18" width="15.125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="11" style="19"/>
+    <col min="20" max="20" width="18" style="19" customWidth="1"/>
+    <col min="21" max="21" width="22.125" style="19" customWidth="1"/>
+    <col min="22" max="22" width="18.875" style="19" customWidth="1"/>
+    <col min="23" max="23" width="15.625" style="19" customWidth="1"/>
+    <col min="24" max="24" width="16" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.5" style="19" customWidth="1"/>
+    <col min="26" max="26" width="23" style="19" customWidth="1"/>
+    <col min="27" max="29" width="16" style="19" customWidth="1"/>
+    <col min="30" max="30" width="25.875" style="19" customWidth="1"/>
+    <col min="31" max="31" width="25.125" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.625" style="19" customWidth="1"/>
+    <col min="33" max="33" width="16.625" style="19" customWidth="1"/>
+    <col min="34" max="34" width="19" style="19" customWidth="1"/>
+    <col min="35" max="36" width="28.875" style="19" customWidth="1"/>
+    <col min="37" max="37" width="14.375" style="19" customWidth="1"/>
+    <col min="38" max="39" width="11" style="19"/>
+    <col min="40" max="42" width="15.5" style="19" customWidth="1"/>
+    <col min="43" max="43" width="16.375" style="19" customWidth="1"/>
+    <col min="44" max="44" width="11" style="19"/>
+    <col min="45" max="45" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="45.375" style="19" customWidth="1"/>
+    <col min="47" max="47" width="11" style="19"/>
+    <col min="48" max="48" width="13.125" style="19" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="34.125" style="19" customWidth="1"/>
+    <col min="50" max="51" width="11" style="19"/>
+    <col min="52" max="52" width="19" style="19" customWidth="1"/>
+    <col min="53" max="53" width="18.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32" style="19" customWidth="1"/>
+    <col min="55" max="16384" width="11" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AY1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="AZ1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BA1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BB1" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="99.75">
-      <c r="A2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="7">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2">
         <v>44603</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="13">
         <v>1.9560185185185184E-2</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="14">
         <v>1.9560185185185184E-2</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="11">
         <v>2011</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="15">
         <v>43585</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="15">
         <v>44680</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="1">
         <v>31028</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AQ2" s="1">
         <v>792853152</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AT2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AU2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AV2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AX2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AY2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BA2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="114">
-      <c r="A3" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="17">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="6">
         <v>44603</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="P3" s="21" t="s">
@@ -1274,7 +1296,7 @@
       <c r="Q3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="7" t="s">
         <v>58</v>
       </c>
       <c r="S3" s="22">
@@ -1286,13 +1308,13 @@
       <c r="U3" s="20">
         <v>2011</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="V3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="W3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="Y3" s="24">
@@ -1301,16 +1323,16 @@
       <c r="Z3" s="24">
         <v>44680</v>
       </c>
-      <c r="AA3" s="18" t="s">
+      <c r="AA3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AB3" s="18">
+      <c r="AB3" s="7">
         <v>31028</v>
       </c>
-      <c r="AC3" s="18" t="s">
+      <c r="AC3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AD3" s="18" t="s">
+      <c r="AD3" s="7" t="s">
         <v>63</v>
       </c>
       <c r="AE3" s="20" t="s">
@@ -1319,7 +1341,7 @@
       <c r="AF3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AG3" s="18" t="s">
+      <c r="AG3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="AH3" s="25" t="s">
@@ -1331,84 +1353,84 @@
       <c r="AJ3" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="AK3" s="18" t="s">
+      <c r="AK3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AL3" s="18" t="s">
+      <c r="AL3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AM3" s="18" t="s">
+      <c r="AM3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AN3" s="18" t="s">
+      <c r="AN3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AO3" s="18" t="s">
+      <c r="AO3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AP3" s="18" t="s">
+      <c r="AP3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AQ3" s="18">
+      <c r="AQ3" s="7">
         <v>79000000</v>
       </c>
-      <c r="AR3" s="18" t="s">
+      <c r="AR3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AS3" s="18" t="s">
+      <c r="AS3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AT3" s="18" t="s">
+      <c r="AT3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="AU3" s="18" t="s">
+      <c r="AU3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AV3" s="18" t="s">
+      <c r="AV3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AW3" s="18" t="s">
+      <c r="AW3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AX3" s="18" t="s">
+      <c r="AX3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AY3" s="18" t="s">
+      <c r="AY3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AZ3" s="18" t="s">
+      <c r="AZ3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="BA3" s="18" t="s">
+      <c r="BA3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="BB3" s="18" t="s">
+      <c r="BB3" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="15" customFormat="1">
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+    <row r="4" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:54" s="15" customFormat="1"/>
-    <row r="6" spans="1:54" s="15" customFormat="1"/>
-    <row r="7" spans="1:54" s="15" customFormat="1"/>
-    <row r="8" spans="1:54" s="15" customFormat="1"/>
-    <row r="9" spans="1:54" s="15" customFormat="1"/>
-    <row r="10" spans="1:54" s="15" customFormat="1"/>
-    <row r="11" spans="1:54" s="15" customFormat="1"/>
-    <row r="12" spans="1:54" s="15" customFormat="1"/>
-    <row r="13" spans="1:54" s="15" customFormat="1"/>
-    <row r="14" spans="1:54" s="15" customFormat="1"/>
-    <row r="15" spans="1:54" s="15" customFormat="1"/>
-    <row r="16" spans="1:54" s="15" customFormat="1"/>
-    <row r="17" s="15" customFormat="1"/>
-    <row r="18" s="15" customFormat="1"/>
-    <row r="19" s="15" customFormat="1"/>
-    <row r="20" s="15" customFormat="1"/>
-    <row r="21" s="15" customFormat="1"/>
-    <row r="22" s="15" customFormat="1"/>
-    <row r="23" s="15" customFormat="1"/>
+    <row r="5" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{140581F9-3987-D049-A4D7-30FD27849327}"/>
@@ -1420,427 +1442,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49817F5C-76B9-F446-AFFD-56DDE9C6A78C}">
-  <dimension ref="A1:BB49"/>
+  <dimension ref="A1:BB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD48"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="16.875" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="21.875" customWidth="1"/>
-    <col min="9" max="9" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.625" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="22.125" customWidth="1"/>
-    <col min="14" max="14" width="28.125" customWidth="1"/>
-    <col min="16" max="17" width="31.625" customWidth="1"/>
-    <col min="18" max="18" width="15.125" customWidth="1"/>
-    <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="21" max="21" width="22.125" customWidth="1"/>
-    <col min="22" max="22" width="18.875" customWidth="1"/>
-    <col min="23" max="23" width="15.625" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.5" customWidth="1"/>
-    <col min="26" max="26" width="23" customWidth="1"/>
-    <col min="27" max="29" width="16" customWidth="1"/>
-    <col min="30" max="30" width="25.875" customWidth="1"/>
-    <col min="31" max="31" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.625" customWidth="1"/>
-    <col min="33" max="33" width="16.625" customWidth="1"/>
-    <col min="34" max="34" width="19" customWidth="1"/>
-    <col min="35" max="36" width="28.875" customWidth="1"/>
-    <col min="37" max="37" width="14.375" customWidth="1"/>
-    <col min="40" max="42" width="15.5" customWidth="1"/>
-    <col min="43" max="43" width="16.375" customWidth="1"/>
-    <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="45.375" customWidth="1"/>
-    <col min="48" max="48" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="34.125" customWidth="1"/>
-    <col min="52" max="52" width="19" customWidth="1"/>
-    <col min="53" max="53" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="32" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="11" style="19"/>
+    <col min="4" max="4" width="13.375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="21" style="19" customWidth="1"/>
+    <col min="6" max="6" width="16.875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="21.875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="22.875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="26" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="19" customWidth="1"/>
+    <col min="13" max="13" width="22.125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="28.125" style="19" customWidth="1"/>
+    <col min="15" max="15" width="11" style="19"/>
+    <col min="16" max="17" width="31.625" style="19" customWidth="1"/>
+    <col min="18" max="18" width="15.125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="11" style="19"/>
+    <col min="20" max="20" width="18" style="19" customWidth="1"/>
+    <col min="21" max="21" width="22.125" style="19" customWidth="1"/>
+    <col min="22" max="22" width="18.875" style="19" customWidth="1"/>
+    <col min="23" max="23" width="15.625" style="19" customWidth="1"/>
+    <col min="24" max="24" width="16" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.5" style="19" customWidth="1"/>
+    <col min="26" max="26" width="23" style="19" customWidth="1"/>
+    <col min="27" max="29" width="16" style="19" customWidth="1"/>
+    <col min="30" max="30" width="25.875" style="19" customWidth="1"/>
+    <col min="31" max="31" width="25.125" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.625" style="19" customWidth="1"/>
+    <col min="33" max="33" width="16.625" style="19" customWidth="1"/>
+    <col min="34" max="34" width="19" style="19" customWidth="1"/>
+    <col min="35" max="36" width="28.875" style="19" customWidth="1"/>
+    <col min="37" max="37" width="14.375" style="19" customWidth="1"/>
+    <col min="38" max="39" width="11" style="19"/>
+    <col min="40" max="42" width="15.5" style="19" customWidth="1"/>
+    <col min="43" max="43" width="16.375" style="19" customWidth="1"/>
+    <col min="44" max="44" width="11" style="19"/>
+    <col min="45" max="45" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="45.375" style="19" customWidth="1"/>
+    <col min="47" max="47" width="11" style="19"/>
+    <col min="48" max="48" width="13.125" style="19" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="34.125" style="19" customWidth="1"/>
+    <col min="50" max="51" width="11" style="19"/>
+    <col min="52" max="52" width="19" style="19" customWidth="1"/>
+    <col min="53" max="53" width="18.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32" style="19" customWidth="1"/>
+    <col min="55" max="16384" width="11" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AY1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="AZ1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BA1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BB1" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="99.75">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>44603</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="13">
         <v>1.9560185185185184E-2</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="14">
         <v>1.9560185185185184E-2</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="11">
         <v>2011</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="15">
         <v>43585</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="15">
         <v>44680</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="1">
         <v>31028</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AQ2" s="1">
         <v>1585642760</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AT2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AU2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AV2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AX2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AY2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BA2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="114">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="6">
         <v>44603</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="P3" s="21" t="s">
@@ -1849,7 +1879,7 @@
       <c r="Q3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="7" t="s">
         <v>58</v>
       </c>
       <c r="S3" s="22">
@@ -1861,13 +1891,13 @@
       <c r="U3" s="20">
         <v>2011</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="V3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="W3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="Y3" s="24">
@@ -1876,16 +1906,16 @@
       <c r="Z3" s="24">
         <v>44680</v>
       </c>
-      <c r="AA3" s="18" t="s">
+      <c r="AA3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AB3" s="18">
+      <c r="AB3" s="7">
         <v>31028</v>
       </c>
-      <c r="AC3" s="18" t="s">
+      <c r="AC3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AD3" s="18" t="s">
+      <c r="AD3" s="7" t="s">
         <v>63</v>
       </c>
       <c r="AE3" s="20" t="s">
@@ -1894,7 +1924,7 @@
       <c r="AF3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AG3" s="18" t="s">
+      <c r="AG3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="AH3" s="25" t="s">
@@ -1906,110 +1936,111 @@
       <c r="AJ3" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="AK3" s="18" t="s">
+      <c r="AK3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AL3" s="18" t="s">
+      <c r="AL3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AM3" s="18" t="s">
+      <c r="AM3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AN3" s="18" t="s">
+      <c r="AN3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AO3" s="18" t="s">
+      <c r="AO3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AP3" s="18" t="s">
+      <c r="AP3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AQ3" s="18">
+      <c r="AQ3" s="7">
         <v>1580000000</v>
       </c>
-      <c r="AR3" s="18" t="s">
+      <c r="AR3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AS3" s="18" t="s">
+      <c r="AS3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="AT3" s="18" t="s">
+      <c r="AT3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AU3" s="18" t="s">
+      <c r="AU3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AV3" s="18" t="s">
+      <c r="AV3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AW3" s="18" t="s">
+      <c r="AW3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AX3" s="18" t="s">
+      <c r="AX3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AY3" s="18" t="s">
+      <c r="AY3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AZ3" s="18" t="s">
+      <c r="AZ3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="BA3" s="18" t="s">
+      <c r="BA3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="BB3" s="18" t="s">
+      <c r="BB3" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="15" customFormat="1">
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+    <row r="4" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:54" s="15" customFormat="1"/>
-    <row r="6" spans="1:54" s="15" customFormat="1"/>
-    <row r="7" spans="1:54" s="15" customFormat="1"/>
-    <row r="8" spans="1:54" s="15" customFormat="1"/>
-    <row r="9" spans="1:54" s="15" customFormat="1"/>
-    <row r="10" spans="1:54" s="15" customFormat="1"/>
-    <row r="11" spans="1:54" s="15" customFormat="1"/>
-    <row r="12" spans="1:54" s="15" customFormat="1"/>
-    <row r="13" spans="1:54" s="15" customFormat="1"/>
-    <row r="14" spans="1:54" s="15" customFormat="1"/>
-    <row r="15" spans="1:54" s="15" customFormat="1"/>
-    <row r="16" spans="1:54" s="15" customFormat="1"/>
-    <row r="17" s="15" customFormat="1"/>
-    <row r="18" s="15" customFormat="1"/>
-    <row r="19" s="15" customFormat="1"/>
-    <row r="20" s="15" customFormat="1"/>
-    <row r="21" s="15" customFormat="1"/>
-    <row r="22" s="15" customFormat="1"/>
-    <row r="23" s="15" customFormat="1"/>
-    <row r="24" s="15" customFormat="1"/>
-    <row r="25" s="15" customFormat="1"/>
-    <row r="26" s="15" customFormat="1"/>
-    <row r="27" s="15" customFormat="1"/>
-    <row r="28" s="15" customFormat="1"/>
-    <row r="29" s="15" customFormat="1"/>
-    <row r="30" s="15" customFormat="1"/>
-    <row r="31" s="15" customFormat="1"/>
-    <row r="32" s="15" customFormat="1"/>
-    <row r="33" s="15" customFormat="1"/>
-    <row r="34" s="15" customFormat="1"/>
-    <row r="35" s="15" customFormat="1"/>
-    <row r="36" s="15" customFormat="1"/>
-    <row r="37" s="15" customFormat="1"/>
-    <row r="38" s="15" customFormat="1"/>
-    <row r="39" s="15" customFormat="1"/>
-    <row r="40" s="15" customFormat="1"/>
-    <row r="41" s="15" customFormat="1"/>
-    <row r="42" s="15" customFormat="1"/>
-    <row r="43" s="15" customFormat="1"/>
-    <row r="44" s="15" customFormat="1"/>
-    <row r="45" s="15" customFormat="1"/>
-    <row r="46" s="15" customFormat="1"/>
-    <row r="47" s="15" customFormat="1"/>
-    <row r="48" s="15" customFormat="1"/>
-    <row r="49" customFormat="1"/>
+    <row r="5" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29"/>
+    </row>
+    <row r="10" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:54" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{1963DBEB-874F-B945-B069-AB9D6469FA57}"/>

</xml_diff>